<commit_message>
treant + shogun updates
</commit_message>
<xml_diff>
--- a/BDD.xlsx
+++ b/BDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Mi unidad\Eras\WEB\visualizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AEE0B8-1244-475A-8861-BAF30B7474C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C070D153-303D-4DF6-8F93-D74E785A50B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2336" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2340" uniqueCount="426">
   <si>
     <t>nombre</t>
   </si>
@@ -1293,6 +1293,24 @@
   </si>
   <si>
     <t>neogeo-shogún</t>
+  </si>
+  <si>
+    <t>Coloso Enraizado</t>
+  </si>
+  <si>
+    <t>treant</t>
+  </si>
+  <si>
+    <t>Bonewillow</t>
+  </si>
+  <si>
+    <t>Treant Courser</t>
+  </si>
+  <si>
+    <t>Siempre Verde</t>
+  </si>
+  <si>
+    <t>treant-vegetación</t>
   </si>
 </sst>
 </file>
@@ -1362,13 +1380,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1673,8 +1692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q521"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A456" workbookViewId="0">
-      <selection activeCell="H473" sqref="H473"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="M217" sqref="M217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6359,7 +6378,7 @@
         <v>121</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>251</v>
+        <v>422</v>
       </c>
       <c r="C123" s="2">
         <v>2</v>
@@ -6376,9 +6395,23 @@
       <c r="G123" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H123" s="3"/>
+      <c r="H123" s="4" t="s">
+        <v>421</v>
+      </c>
       <c r="I123" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
+      </c>
+      <c r="J123" s="2">
+        <v>2</v>
+      </c>
+      <c r="K123" s="2">
+        <v>6</v>
+      </c>
+      <c r="L123" s="2">
+        <v>2</v>
+      </c>
+      <c r="M123" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
@@ -6636,7 +6669,7 @@
         <v>129</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>251</v>
+        <v>420</v>
       </c>
       <c r="C131" s="2">
         <v>2</v>
@@ -6653,8 +6686,23 @@
       <c r="G131" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="H131" s="2" t="s">
+        <v>421</v>
+      </c>
       <c r="I131" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
+      </c>
+      <c r="J131" s="2">
+        <v>2</v>
+      </c>
+      <c r="K131" s="2">
+        <v>5</v>
+      </c>
+      <c r="L131" s="2">
+        <v>2</v>
+      </c>
+      <c r="M131" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
@@ -9096,7 +9144,7 @@
         <v>202</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>251</v>
+        <v>423</v>
       </c>
       <c r="C204" s="2">
         <v>3</v>
@@ -9113,8 +9161,23 @@
       <c r="G204" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="H204" s="2" t="s">
+        <v>421</v>
+      </c>
       <c r="I204" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
+      </c>
+      <c r="J204" s="2">
+        <v>3</v>
+      </c>
+      <c r="K204" s="2">
+        <v>9</v>
+      </c>
+      <c r="L204" s="2">
+        <v>3</v>
+      </c>
+      <c r="M204" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.25">
@@ -9546,7 +9609,7 @@
         <v>215</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>251</v>
+        <v>424</v>
       </c>
       <c r="C217" s="2">
         <v>3</v>
@@ -9563,8 +9626,17 @@
       <c r="G217" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="H217" s="2" t="s">
+        <v>425</v>
+      </c>
       <c r="I217" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
+      </c>
+      <c r="J217" s="2">
+        <v>2</v>
+      </c>
+      <c r="L217" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>